<commit_message>
Backup QR Scanner data - 05/04/2025, 21:21:51
</commit_message>
<xml_diff>
--- a/backups/qr_scanner_backup_20250405_2121.xlsx
+++ b/backups/qr_scanner_backup_20250405_2121.xlsx
@@ -4,6 +4,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="lolo" sheetId="1" r:id="rId1"/>
+    <sheet name="ghkn" sheetId="2" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
@@ -441,4 +442,52 @@
     <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Number</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Student ID</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Location</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Log Date</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Log Time</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="str">
+        <v>dfvk</v>
+      </c>
+      <c r="C2" t="str">
+        <v>ghkn</v>
+      </c>
+      <c r="D2" t="str">
+        <v>2025-04-05</v>
+      </c>
+      <c r="E2" t="str">
+        <v>21:21:45</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>